<commit_message>
commit before remote repo setup
</commit_message>
<xml_diff>
--- a/docs/county_mapping_tbl.xlsx
+++ b/docs/county_mapping_tbl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rawatsa\OneDrive - University of Cincinnati\SASprojects\ohphs_covid_impact\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{5122DB29-CB47-40FE-AE4D-D6A7324EA1E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BF7127C0-D5A0-4844-B428-3F123B3E332B}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{5122DB29-CB47-40FE-AE4D-D6A7324EA1E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{19BF9520-74A7-4BAC-9BE3-EB9875226F4D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{25520D71-C464-4516-88D5-633C8364372E}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="read_me" sheetId="2" r:id="rId1"/>
     <sheet name="mapping" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mapping!$A$1:$D$89</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="102">
   <si>
     <t>county_num</t>
   </si>
@@ -323,6 +326,15 @@
   </si>
   <si>
     <t xml:space="preserve">wyandot </t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>urban</t>
+  </si>
+  <si>
+    <t>rural</t>
   </si>
 </sst>
 </file>
@@ -739,10 +751,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3556A2E7-9620-4891-8EF1-E9CC6AD9979C}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +764,7 @@
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -762,8 +774,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -774,8 +789,11 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -786,8 +804,11 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -798,8 +819,11 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -810,8 +834,11 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -822,8 +849,11 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -834,8 +864,11 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -846,8 +879,11 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -858,8 +894,11 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -870,8 +909,11 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -882,8 +924,11 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -894,8 +939,11 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -906,8 +954,11 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -918,8 +969,11 @@
       <c r="C14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -930,8 +984,11 @@
       <c r="C15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -942,8 +999,11 @@
       <c r="C16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -954,8 +1014,11 @@
       <c r="C17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -966,8 +1029,11 @@
       <c r="C18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -978,8 +1044,11 @@
       <c r="C19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -990,8 +1059,11 @@
       <c r="C20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1002,8 +1074,11 @@
       <c r="C21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1014,8 +1089,11 @@
       <c r="C22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1026,8 +1104,11 @@
       <c r="C23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1038,8 +1119,11 @@
       <c r="C24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1050,8 +1134,11 @@
       <c r="C25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1062,8 +1149,11 @@
       <c r="C26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1074,8 +1164,11 @@
       <c r="C27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1086,8 +1179,11 @@
       <c r="C28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1098,8 +1194,11 @@
       <c r="C29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1110,8 +1209,11 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1122,8 +1224,11 @@
       <c r="C31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1134,8 +1239,11 @@
       <c r="C32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1146,8 +1254,11 @@
       <c r="C33" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1158,8 +1269,11 @@
       <c r="C34" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1170,8 +1284,11 @@
       <c r="C35" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1182,8 +1299,11 @@
       <c r="C36" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1194,8 +1314,11 @@
       <c r="C37" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1206,8 +1329,11 @@
       <c r="C38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1218,8 +1344,11 @@
       <c r="C39" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1230,8 +1359,11 @@
       <c r="C40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1242,8 +1374,11 @@
       <c r="C41" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1254,8 +1389,11 @@
       <c r="C42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1266,8 +1404,11 @@
       <c r="C43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1278,8 +1419,11 @@
       <c r="C44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1290,8 +1434,11 @@
       <c r="C45" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1302,8 +1449,11 @@
       <c r="C46" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1314,8 +1464,11 @@
       <c r="C47" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1326,8 +1479,11 @@
       <c r="C48" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1338,8 +1494,11 @@
       <c r="C49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1350,8 +1509,11 @@
       <c r="C50" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1362,8 +1524,11 @@
       <c r="C51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1374,8 +1539,11 @@
       <c r="C52" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1386,8 +1554,11 @@
       <c r="C53" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1398,8 +1569,11 @@
       <c r="C54" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1410,8 +1584,11 @@
       <c r="C55" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1422,8 +1599,11 @@
       <c r="C56" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1434,8 +1614,11 @@
       <c r="C57" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1446,8 +1629,11 @@
       <c r="C58" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1458,8 +1644,11 @@
       <c r="C59" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1470,8 +1659,11 @@
       <c r="C60" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1482,8 +1674,11 @@
       <c r="C61" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1494,8 +1689,11 @@
       <c r="C62" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1506,8 +1704,11 @@
       <c r="C63" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1518,8 +1719,11 @@
       <c r="C64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1530,8 +1734,11 @@
       <c r="C65" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1542,8 +1749,11 @@
       <c r="C66" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1554,8 +1764,11 @@
       <c r="C67" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1566,8 +1779,11 @@
       <c r="C68" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1578,8 +1794,11 @@
       <c r="C69" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1590,8 +1809,11 @@
       <c r="C70" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1602,8 +1824,11 @@
       <c r="C71" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1614,8 +1839,11 @@
       <c r="C72" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1626,8 +1854,11 @@
       <c r="C73" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1638,8 +1869,11 @@
       <c r="C74" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1650,8 +1884,11 @@
       <c r="C75" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1662,8 +1899,11 @@
       <c r="C76" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1674,8 +1914,11 @@
       <c r="C77" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1686,8 +1929,11 @@
       <c r="C78" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1698,8 +1944,11 @@
       <c r="C79" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1710,8 +1959,11 @@
       <c r="C80" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1722,8 +1974,11 @@
       <c r="C81" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1734,8 +1989,11 @@
       <c r="C82" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1746,8 +2004,11 @@
       <c r="C83" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1758,8 +2019,11 @@
       <c r="C84" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1770,8 +2034,11 @@
       <c r="C85" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1782,8 +2049,11 @@
       <c r="C86" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1794,8 +2064,11 @@
       <c r="C87" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1806,8 +2079,11 @@
       <c r="C88" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1817,6 +2093,9 @@
       </c>
       <c r="C89" t="s">
         <v>98</v>
+      </c>
+      <c r="D89" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1831,15 +2110,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060C37653FBFDB34DA291AE7806E480FB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f94e6187d2db220b108a9f3f0e9620ab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9772973a-2681-4778-b4c7-fa785e6ae870" xmlns:ns4="bb53d160-e9b7-42e4-9639-85c2eeb2a294" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="319ae0e8b2240766e8bd2072e6b672dc" ns3:_="" ns4:_="">
     <xsd:import namespace="9772973a-2681-4778-b4c7-fa785e6ae870"/>
@@ -2068,32 +2338,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5A9BA0F-1149-4B20-A032-010A3E49DCC4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="9772973a-2681-4778-b4c7-fa785e6ae870"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="bb53d160-e9b7-42e4-9639-85c2eeb2a294"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3DD7C0E-86FE-4DB1-BE9F-357566DACA83}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92D8EB69-D5F4-4A60-88C3-3E41B01B3289}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2110,4 +2381,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3DD7C0E-86FE-4DB1-BE9F-357566DACA83}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>